<commit_message>
Added forgot pasword tests
</commit_message>
<xml_diff>
--- a/target/classes/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/target/classes/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AD7284-5653-4E8F-B6E0-78B8BF9B1C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B5AEE-FE76-42AB-BE9D-FD9445BEB05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{9B270448-1A92-4C34-AABB-F2D6A45C5F02}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -48,18 +48,6 @@
   </si>
   <si>
     <t>test@123</t>
-  </si>
-  <si>
-    <t>sads@asdas.com</t>
-  </si>
-  <si>
-    <t>sdw323</t>
-  </si>
-  <si>
-    <t>sgy3@vcf.com</t>
-  </si>
-  <si>
-    <t>yyguy234t</t>
   </si>
 </sst>
 </file>
@@ -147,12 +135,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -468,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F784E2C6-D5DE-48DA-8E3F-8BD93FFE66DF}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,30 +482,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{DD2CD233-EBEE-40B6-92C4-85465AC12666}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{64D1CBFB-7E13-4FE1-8403-163E395966C4}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{D4131ED5-AE16-48B2-B184-C9C4AF540614}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>